<commit_message>
Applied chages and verified the execution
</commit_message>
<xml_diff>
--- a/Automation/Login_Folder/Login_Data.xlsx
+++ b/Automation/Login_Folder/Login_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bssuniversal-my.sharepoint.com/personal/laraib_khalid_bssuniversal_com/Documents/Desktop/Laraib Data/SQA/Automation/DemoSMARTCRM/Automation/Login_Folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abubakar.Arshad\PycharmProjects\Demo_SmartCRM-Final\Automation\Login_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_F25DC773A252ABDACC10480271DD697A5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8420FFBB-A9D2-4F43-A097-F3AED01CB4A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923ED453-F6D6-436B-A538-5BA7E6B333E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31350" yWindow="1215" windowWidth="16830" windowHeight="10575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>${username}</t>
   </si>
@@ -373,19 +373,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -393,35 +393,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>123</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated automation test cases
</commit_message>
<xml_diff>
--- a/Automation/Login_Folder/Login_Data.xlsx
+++ b/Automation/Login_Folder/Login_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abubakar.Arshad\PycharmProjects\Demo_SmartCRM-Final\Automation\Login_Folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmad.Raza\PycharmProjects\Demo_SmartCRM-Final\Automation\Login_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923ED453-F6D6-436B-A538-5BA7E6B333E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B579044-ECB1-4723-96E5-F6C3BD3BACBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31350" yWindow="1215" windowWidth="16830" windowHeight="10575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>${username}</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Bss@2025-1</t>
+  </si>
+  <si>
+    <t>${Status}</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Valid</t>
   </si>
 </sst>
 </file>
@@ -373,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,36 +394,48 @@
     <col min="2" max="2" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>123</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>